<commit_message>
Updated For Email Template
</commit_message>
<xml_diff>
--- a/Data/OtherTemplates/MsPayroll_WorkLog.xlsx
+++ b/Data/OtherTemplates/MsPayroll_WorkLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WORKSTATION-VM\Documents\UiPath\moneysoft-payroll-basic\Data\OtherTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD3A49B-2D38-404F-B939-BBD778D9B697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83EB8BC-F682-49A1-86D6-11F7F2AD1AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="9015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>COMPANY_NAME</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>REMARK</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -384,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,6 +430,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Secound UTA test commit
</commit_message>
<xml_diff>
--- a/Data/OtherTemplates/MsPayroll_WorkLog.xlsx
+++ b/Data/OtherTemplates/MsPayroll_WorkLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WORKSTATION-VM\Documents\UiPath\moneysoft-payroll-basic\Data\OtherTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D041AF-736E-4136-A605-735E4F9A2145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30A6815-20E1-4071-B1B7-8B42995DB598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="9015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,8 +386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>